<commit_message>
validating look up table
added code for checking the KDR when look up table is used
</commit_message>
<xml_diff>
--- a/Optimal_parameters.xlsx
+++ b/Optimal_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cp17593\SYNERGIA\Python_codes\Secret_Key_sharing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E5DF04D-5B47-4C50-AD6E-2F9B4C573458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFD8C00-00D4-43CA-95D7-6CAC276E3D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4BEEE29-95E0-4859-9DA9-01C1A6B60363}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4BEEE29-95E0-4859-9DA9-01C1A6B60363}"/>
   </bookViews>
   <sheets>
     <sheet name="KDR&lt;0.001" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t xml:space="preserve">channel missmatch (p_ch) </t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>Enter L_fkey:</t>
+  </si>
+  <si>
+    <t>tau</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>pch</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -147,13 +159,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>550545</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>110490</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -1260,11 +1272,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0F4A94-E674-46B3-8348-963C26630677}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,33 +1285,33 @@
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.01</v>
       </c>
@@ -1312,16 +1324,16 @@
       <c r="D2" s="2">
         <v>0.49009999999999998</v>
       </c>
+      <c r="E2">
+        <f>_xlfn.CEILING.MATH(I3/(B2*D2))</f>
+        <v>9</v>
+      </c>
       <c r="F2">
-        <f>_xlfn.CEILING.MATH(J3/(B2*D2))</f>
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <f>F2*B2</f>
+        <f>E2*B2</f>
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.02</v>
       </c>
@@ -1334,22 +1346,22 @@
       <c r="D3" s="2">
         <v>0.48039999999999999</v>
       </c>
+      <c r="E3">
+        <f>_xlfn.CEILING.MATH(I3/(B3*D3))</f>
+        <v>9</v>
+      </c>
       <c r="F3">
-        <f>_xlfn.CEILING.MATH(J3/(B3*D3))</f>
-        <v>9</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G31" si="0">F3*B3</f>
+        <f>E3*B3</f>
         <v>18</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="3">
+      <c r="I3" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.03</v>
       </c>
@@ -1362,16 +1374,16 @@
       <c r="D4" s="2">
         <v>0.47089999999999999</v>
       </c>
+      <c r="E4">
+        <f>_xlfn.CEILING.MATH(I3/(B4*D4))</f>
+        <v>9</v>
+      </c>
       <c r="F4">
-        <f>_xlfn.CEILING.MATH(J3/(B4*D4))</f>
-        <v>9</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
+        <f>E4*B4</f>
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.04</v>
       </c>
@@ -1384,16 +1396,16 @@
       <c r="D5" s="2">
         <v>0.2949</v>
       </c>
+      <c r="E5">
+        <f>_xlfn.CEILING.MATH(I3/(B5*D5))</f>
+        <v>10</v>
+      </c>
       <c r="F5">
-        <f>_xlfn.CEILING.MATH(J3/(B5*D5))</f>
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
+        <f>E5*B5</f>
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.05</v>
       </c>
@@ -1406,16 +1418,16 @@
       <c r="D6" s="2">
         <v>0.2858</v>
       </c>
+      <c r="E6">
+        <f>_xlfn.CEILING.MATH(I3/(B6*D6))</f>
+        <v>10</v>
+      </c>
       <c r="F6">
-        <f>_xlfn.CEILING.MATH(J3/(B6*D6))</f>
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
+        <f>E6*B6</f>
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.06</v>
       </c>
@@ -1428,16 +1440,16 @@
       <c r="D7" s="2">
         <v>0.27689999999999998</v>
       </c>
+      <c r="E7">
+        <f>_xlfn.CEILING.MATH(I3/(B7*D7))</f>
+        <v>10</v>
+      </c>
       <c r="F7">
-        <f>_xlfn.CEILING.MATH(J3/(B7*D7))</f>
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
+        <f>E7*B7</f>
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -1450,16 +1462,16 @@
       <c r="D8" s="2">
         <v>0.26819999999999999</v>
       </c>
+      <c r="E8">
+        <f>_xlfn.CEILING.MATH(I3/(B8*D8))</f>
+        <v>10</v>
+      </c>
       <c r="F8">
-        <f>_xlfn.CEILING.MATH(J3/(B8*D8))</f>
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
+        <f>E8*B8</f>
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.08</v>
       </c>
@@ -1472,16 +1484,16 @@
       <c r="D9" s="2">
         <v>0.25969999999999999</v>
       </c>
+      <c r="E9">
+        <f>_xlfn.CEILING.MATH(I3/(B9*D9))</f>
+        <v>11</v>
+      </c>
       <c r="F9">
-        <f>_xlfn.CEILING.MATH(J3/(B9*D9))</f>
-        <v>11</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
+        <f>E9*B9</f>
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.09</v>
       </c>
@@ -1494,16 +1506,16 @@
       <c r="D10" s="2">
         <v>0.25140000000000001</v>
       </c>
+      <c r="E10">
+        <f>_xlfn.CEILING.MATH(I3/(B10*D10))</f>
+        <v>11</v>
+      </c>
       <c r="F10">
-        <f>_xlfn.CEILING.MATH(J3/(B10*D10))</f>
-        <v>11</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
+        <f>E10*B10</f>
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.1</v>
       </c>
@@ -1516,16 +1528,16 @@
       <c r="D11" s="2">
         <v>0.18379999999999999</v>
       </c>
+      <c r="E11">
+        <f>_xlfn.CEILING.MATH(I3/(B11*D11))</f>
+        <v>9</v>
+      </c>
       <c r="F11">
-        <f>_xlfn.CEILING.MATH(J3/(B11*D11))</f>
-        <v>9</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
+        <f>E11*B11</f>
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.11</v>
       </c>
@@ -1538,16 +1550,16 @@
       <c r="D12" s="2">
         <v>0.18079999999999999</v>
       </c>
+      <c r="E12">
+        <f>_xlfn.CEILING.MATH(I3/(B12*D12))</f>
+        <v>9</v>
+      </c>
       <c r="F12">
-        <f>_xlfn.CEILING.MATH(J3/(B12*D12))</f>
-        <v>9</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
+        <f>E12*B12</f>
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.12</v>
       </c>
@@ -1560,16 +1572,16 @@
       <c r="D13" s="2">
         <v>0.15</v>
       </c>
+      <c r="E13">
+        <f>_xlfn.CEILING.MATH(I3/(B13*D13))</f>
+        <v>14</v>
+      </c>
       <c r="F13">
-        <f>_xlfn.CEILING.MATH(J3/(B13*D13))</f>
-        <v>14</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
+        <f>E13*B13</f>
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.13</v>
       </c>
@@ -1582,16 +1594,16 @@
       <c r="D14" s="2">
         <v>0.14330000000000001</v>
       </c>
+      <c r="E14">
+        <f>_xlfn.CEILING.MATH(I3/(B14*D14))</f>
+        <v>14</v>
+      </c>
       <c r="F14">
-        <f>_xlfn.CEILING.MATH(J3/(B14*D14))</f>
-        <v>14</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
+        <f>E14*B14</f>
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.14000000000000001</v>
       </c>
@@ -1604,16 +1616,16 @@
       <c r="D15" s="2">
         <v>0.1368</v>
       </c>
+      <c r="E15">
+        <f>_xlfn.CEILING.MATH(I3/(B15*D15))</f>
+        <v>15</v>
+      </c>
       <c r="F15">
-        <f>_xlfn.CEILING.MATH(J3/(B15*D15))</f>
-        <v>15</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
+        <f>E15*B15</f>
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.15</v>
       </c>
@@ -1626,16 +1638,16 @@
       <c r="D16" s="2">
         <v>0.13059999999999999</v>
       </c>
+      <c r="E16">
+        <f>_xlfn.CEILING.MATH(I3/(B16*D16))</f>
+        <v>16</v>
+      </c>
       <c r="F16">
-        <f>_xlfn.CEILING.MATH(J3/(B16*D16))</f>
-        <v>16</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
+        <f>E16*B16</f>
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.16</v>
       </c>
@@ -1648,16 +1660,16 @@
       <c r="D17" s="2">
         <v>0.12559999999999999</v>
       </c>
+      <c r="E17">
+        <f>_xlfn.CEILING.MATH(I3/(B17*D17))</f>
+        <v>11</v>
+      </c>
       <c r="F17">
-        <f>_xlfn.CEILING.MATH(J3/(B17*D17))</f>
-        <v>11</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="0"/>
+        <f>E17*B17</f>
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.17</v>
       </c>
@@ -1670,16 +1682,16 @@
       <c r="D18" s="2">
         <v>0.1074</v>
       </c>
+      <c r="E18">
+        <f>_xlfn.CEILING.MATH(I3/(B18*D18))</f>
+        <v>10</v>
+      </c>
       <c r="F18">
-        <f>_xlfn.CEILING.MATH(J3/(B18*D18))</f>
-        <v>10</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="0"/>
+        <f>E18*B18</f>
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.18</v>
       </c>
@@ -1692,16 +1704,16 @@
       <c r="D19" s="2">
         <v>0.105</v>
       </c>
+      <c r="E19">
+        <f>_xlfn.CEILING.MATH(I3/(B19*D19))</f>
+        <v>10</v>
+      </c>
       <c r="F19">
-        <f>_xlfn.CEILING.MATH(J3/(B19*D19))</f>
-        <v>10</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
+        <f>E19*B19</f>
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.19</v>
       </c>
@@ -1714,16 +1726,16 @@
       <c r="D20" s="2">
         <v>8.9700000000000002E-2</v>
       </c>
+      <c r="E20">
+        <f>_xlfn.CEILING.MATH(I3/(B20*D20))</f>
+        <v>9</v>
+      </c>
       <c r="F20">
-        <f>_xlfn.CEILING.MATH(J3/(B20*D20))</f>
-        <v>9</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="0"/>
+        <f>E20*B20</f>
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.2</v>
       </c>
@@ -1736,16 +1748,16 @@
       <c r="D21" s="2">
         <v>8.7999999999999995E-2</v>
       </c>
+      <c r="E21">
+        <f>_xlfn.CEILING.MATH(I3/(B21*D21))</f>
+        <v>10</v>
+      </c>
       <c r="F21">
-        <f>_xlfn.CEILING.MATH(J3/(B21*D21))</f>
-        <v>10</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="0"/>
+        <f>E21*B21</f>
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.21</v>
       </c>
@@ -1758,16 +1770,16 @@
       <c r="D22" s="2">
         <v>7.9100000000000004E-2</v>
       </c>
+      <c r="E22">
+        <f>_xlfn.CEILING.MATH(I3/(B22*D22))</f>
+        <v>12</v>
+      </c>
       <c r="F22">
-        <f>_xlfn.CEILING.MATH(J3/(B22*D22))</f>
-        <v>12</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="0"/>
+        <f>E22*B22</f>
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.22</v>
       </c>
@@ -1780,16 +1792,16 @@
       <c r="D23" s="2">
         <v>7.6100000000000001E-2</v>
       </c>
+      <c r="E23">
+        <f>_xlfn.CEILING.MATH(I3/(B23*D23))</f>
+        <v>12</v>
+      </c>
       <c r="F23">
-        <f>_xlfn.CEILING.MATH(J3/(B23*D23))</f>
-        <v>12</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="0"/>
+        <f>E23*B23</f>
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.23</v>
       </c>
@@ -1802,16 +1814,16 @@
       <c r="D24" s="2">
         <v>6.9800000000000001E-2</v>
       </c>
+      <c r="E24">
+        <f>_xlfn.CEILING.MATH(I3/(B24*D24))</f>
+        <v>11</v>
+      </c>
       <c r="F24">
-        <f>_xlfn.CEILING.MATH(J3/(B24*D24))</f>
-        <v>11</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="0"/>
+        <f>E24*B24</f>
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.24</v>
       </c>
@@ -1824,16 +1836,16 @@
       <c r="D25" s="2">
         <v>6.3E-2</v>
       </c>
+      <c r="E25">
+        <f>_xlfn.CEILING.MATH(I3/(B25*D25))</f>
+        <v>10</v>
+      </c>
       <c r="F25">
-        <f>_xlfn.CEILING.MATH(J3/(B25*D25))</f>
-        <v>10</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="0"/>
+        <f>E25*B25</f>
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.25</v>
       </c>
@@ -1846,16 +1858,16 @@
       <c r="D26" s="2">
         <v>5.6800000000000003E-2</v>
       </c>
+      <c r="E26">
+        <f>_xlfn.CEILING.MATH(I3/(B26*D26))</f>
+        <v>10</v>
+      </c>
       <c r="F26">
-        <f>_xlfn.CEILING.MATH(J3/(B26*D26))</f>
-        <v>10</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="0"/>
+        <f>E26*B26</f>
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.26</v>
       </c>
@@ -1868,16 +1880,16 @@
       <c r="D27" s="2">
         <v>5.1499999999999997E-2</v>
       </c>
+      <c r="E27">
+        <f>_xlfn.CEILING.MATH(I3/(B27*D27))</f>
+        <v>13</v>
+      </c>
       <c r="F27">
-        <f>_xlfn.CEILING.MATH(J3/(B27*D27))</f>
-        <v>13</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="0"/>
+        <f>E27*B27</f>
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0.27</v>
       </c>
@@ -1890,16 +1902,16 @@
       <c r="D28" s="2">
         <v>4.87E-2</v>
       </c>
+      <c r="E28">
+        <f>_xlfn.CEILING.MATH(I3/(B28*D28))</f>
+        <v>12</v>
+      </c>
       <c r="F28">
-        <f>_xlfn.CEILING.MATH(J3/(B28*D28))</f>
-        <v>12</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="0"/>
+        <f>E28*B28</f>
         <v>168</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.28000000000000003</v>
       </c>
@@ -1912,16 +1924,16 @@
       <c r="D29" s="2">
         <v>4.3499999999999997E-2</v>
       </c>
+      <c r="E29">
+        <f>_xlfn.CEILING.MATH(I3/(B29*D29))</f>
+        <v>11</v>
+      </c>
       <c r="F29">
-        <f>_xlfn.CEILING.MATH(J3/(B29*D29))</f>
-        <v>11</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="0"/>
+        <f>E29*B29</f>
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.28999999999999998</v>
       </c>
@@ -1934,16 +1946,16 @@
       <c r="D30" s="2">
         <v>3.8300000000000001E-2</v>
       </c>
+      <c r="E30">
+        <f>_xlfn.CEILING.MATH(I3/(B30*D30))</f>
+        <v>10</v>
+      </c>
       <c r="F30">
-        <f>_xlfn.CEILING.MATH(J3/(B30*D30))</f>
-        <v>10</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="0"/>
+        <f>E30*B30</f>
         <v>220</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.3</v>
       </c>
@@ -1956,16 +1968,16 @@
       <c r="D31" s="2">
         <v>3.5099999999999999E-2</v>
       </c>
+      <c r="E31">
+        <f>_xlfn.CEILING.MATH(I3/(B31*D31))</f>
+        <v>12</v>
+      </c>
       <c r="F31">
-        <f>_xlfn.CEILING.MATH(J3/(B31*D31))</f>
-        <v>12</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="0"/>
+        <f>E31*B31</f>
         <v>228</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
@@ -1985,7 +1997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B89DAEB-B7FE-4A30-B88C-9297A1926C6D}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>

</xml_diff>